<commit_message>
Updated Feature Extraction code and relabeled song ids
</commit_message>
<xml_diff>
--- a/Data/FirstVerseTimes.xlsx
+++ b/Data/FirstVerseTimes.xlsx
@@ -777,7 +777,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -817,20 +817,20 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>3030</v>
+      <c r="B2" t="s">
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E2">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="F2">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -841,19 +841,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="E3">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F3">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
@@ -864,19 +864,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="E4">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F4">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -887,19 +887,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E5">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F5">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
@@ -910,19 +910,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E6">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F6">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
@@ -933,19 +933,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E7">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F7">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
@@ -956,24 +956,21 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8">
+        <v>23</v>
+      </c>
+      <c r="F8">
         <v>78</v>
       </c>
-      <c r="C8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8">
-        <v>29</v>
-      </c>
-      <c r="F8">
-        <v>166</v>
-      </c>
       <c r="G8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
         <v>0</v>
       </c>
     </row>
@@ -982,19 +979,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E9">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
@@ -1005,19 +1002,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E10">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F10">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="G10" t="s">
         <v>0</v>
@@ -1028,19 +1025,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
         <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11">
-        <v>46</v>
-      </c>
-      <c r="F11">
-        <v>87</v>
       </c>
       <c r="G11" t="s">
         <v>0</v>
@@ -1051,19 +1048,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
         <v>65</v>
-      </c>
-      <c r="D12" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12">
-        <v>21</v>
-      </c>
-      <c r="F12">
-        <v>80</v>
       </c>
       <c r="G12" t="s">
         <v>0</v>
@@ -1074,19 +1071,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="E13">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
         <v>0</v>
@@ -1097,24 +1094,21 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F14">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1123,19 +1117,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E15">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="F15">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
         <v>0</v>
@@ -1145,25 +1139,22 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>74</v>
+      <c r="B16" s="1">
+        <v>3030</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="F16">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="G16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1172,16 +1163,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E17">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F17">
         <v>88</v>
@@ -1195,24 +1186,21 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E18">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F18">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1221,19 +1209,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E19">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F19">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
         <v>0</v>
@@ -1244,19 +1232,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E20">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F20">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="G20" t="s">
         <v>0</v>
@@ -1267,19 +1255,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="E21">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F21">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="G21" t="s">
         <v>0</v>
@@ -1290,19 +1278,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="E22">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F22">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="G22" t="s">
         <v>0</v>
@@ -1313,19 +1301,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="E23">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F23">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="G23" t="s">
         <v>0</v>
@@ -1336,19 +1324,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="E24">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="F24">
-        <v>123</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
         <v>0</v>
@@ -1359,19 +1347,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="E25">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F25">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="G25" t="s">
         <v>0</v>
@@ -1382,19 +1370,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="E26">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F26">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="G26" t="s">
         <v>0</v>
@@ -1405,19 +1393,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E27">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F27">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G27" t="s">
         <v>0</v>
@@ -1428,19 +1416,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="E28">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F28">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G28" t="s">
         <v>0</v>
@@ -1451,21 +1439,24 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E29">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F29">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1474,19 +1465,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E30">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F30">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G30" t="s">
         <v>0</v>
@@ -1497,19 +1488,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E31">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F31">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="G31" t="s">
         <v>0</v>
@@ -1520,21 +1511,24 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="E32">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F32">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="G32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1543,21 +1537,24 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="E33">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F33">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="G33" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1566,21 +1563,24 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E34">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="F34">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1589,19 +1589,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="E35">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F35">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="G35" t="s">
         <v>0</v>
@@ -1612,19 +1612,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="E36">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F36">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G36" t="s">
         <v>0</v>
@@ -1635,19 +1635,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="E37">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F37">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G37" t="s">
         <v>0</v>
@@ -1658,21 +1658,24 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E38">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F38">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="G38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1681,24 +1684,21 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="E39">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F39">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G39" t="s">
-        <v>0</v>
-      </c>
-      <c r="H39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1707,21 +1707,24 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="F40">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="G40" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1730,24 +1733,21 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="D41" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="E41">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F41">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="G41" t="s">
-        <v>0</v>
-      </c>
-      <c r="H41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1756,19 +1756,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E42">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="F42">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="G42" t="s">
         <v>0</v>
@@ -1776,7 +1776,7 @@
     </row>
   </sheetData>
   <sortState ref="B2:H42">
-    <sortCondition ref="B2:B42"/>
+    <sortCondition ref="C2:C42"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>